<commit_message>
Put device_id (url) in actuator specifiers.
</commit_message>
<xml_diff>
--- a/pub-jaen/jaen/schema_gen/openc2_genj.xlsx
+++ b/pub-jaen/jaen/schema_gen/openc2_genj.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="598">
   <si>
-    <t>Generated from schema\openc2.jaen, Mon Mar 27 15:17:55 2017</t>
+    <t>Generated from schema\openc2.jaen, Mon Mar 27 15:57:46 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -141,7 +141,7 @@
     <t>device-id (String)</t>
   </si>
   <si>
-    <t>ID of the command issuer, from "command-src" modifier</t>
+    <t>ID of the command issuer, from "command_src" modifier</t>
   </si>
   <si>
     <t>command_ref (required)</t>
@@ -150,7 +150,7 @@
     <t>command-id (String)</t>
   </si>
   <si>
-    <t>Command unique identifier, from "command-id" modifier</t>
+    <t>Command unique identifier, from "command_id" modifier</t>
   </si>
   <si>
     <t>status (required)</t>
@@ -603,7 +603,7 @@
     <t>ActuatorSpecifiers</t>
   </si>
   <si>
-    <t>port (optional)</t>
+    <t>device_id (optional)</t>
   </si>
   <si>
     <t>asset_id (optional)</t>
@@ -696,7 +696,7 @@
     <t>where (vocab)</t>
   </si>
   <si>
-    <t>allow, deny, contain, allow</t>
+    <t>allow, deny, contain</t>
   </si>
   <si>
     <t>message (optional)</t>
@@ -750,7 +750,7 @@
     <t>device-id</t>
   </si>
   <si>
-    <t>Device Identifier / Address</t>
+    <t>Device Identifier / Address (url)</t>
   </si>
   <si>
     <t>response-type</t>
@@ -3605,7 +3605,7 @@
         <v>195</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="E124" s="8"/>
     </row>
@@ -3749,7 +3749,7 @@
         <v>210</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
Add Symantec use cases, fix missing optional in hashes-type
</commit_message>
<xml_diff>
--- a/pub-jaen/jaen/schema_gen/openc2_genj.xlsx
+++ b/pub-jaen/jaen/schema_gen/openc2_genj.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="756">
   <si>
-    <t>Generated from schema\openc2.jaen, Mon Apr 10 13:29:06 2017</t>
+    <t>Generated from schema\openc2.jaen, Tue Apr 11 09:49:57 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -1056,7 +1056,7 @@
     <t>Hash values for algorithms included in hash-algo-ov</t>
   </si>
   <si>
-    <t>MD5 (required)</t>
+    <t>MD5 (optional)</t>
   </si>
   <si>
     <t>Hex (String)</t>
@@ -1065,79 +1065,79 @@
     <t>MD5 message digest as defined in RFC3121</t>
   </si>
   <si>
-    <t>MD6 (required)</t>
+    <t>MD6 (optional)</t>
   </si>
   <si>
     <t>MD6 message digest as defined in MD6 proposal</t>
   </si>
   <si>
-    <t>RIPEMD-160 (required)</t>
+    <t>RIPEMD-160 (optional)</t>
   </si>
   <si>
     <t>RACE Integrity Primitives Evaluation Message as defined in RIPEMD-160 specification</t>
   </si>
   <si>
-    <t>SHA-1 (required)</t>
+    <t>SHA-1 (optional)</t>
   </si>
   <si>
     <t>Secure Hash Algorithm (SHA)-1 as defined in RFC3174</t>
   </si>
   <si>
-    <t>SHA-224 (required)</t>
+    <t>SHA-224 (optional)</t>
   </si>
   <si>
     <t>SHA-224 as defined in RFC6234 (US Secure Hash Algorithms)</t>
   </si>
   <si>
-    <t>SHA-256 (required)</t>
+    <t>SHA-256 (optional)</t>
   </si>
   <si>
     <t>SHA-256 as defined in RFC6234</t>
   </si>
   <si>
-    <t>SHA-384 (required)</t>
+    <t>SHA-384 (optional)</t>
   </si>
   <si>
     <t>SHA-384 as defined in RFC6234</t>
   </si>
   <si>
-    <t>SHA-512 (required)</t>
+    <t>SHA-512 (optional)</t>
   </si>
   <si>
     <t>SHA-512 as defined in RFC6234</t>
   </si>
   <si>
-    <t>SHA3-224 (required)</t>
+    <t>SHA3-224 (optional)</t>
   </si>
   <si>
     <t>SHA3-224 as defined in FIPS PUP 202</t>
   </si>
   <si>
-    <t>SHA3-256 (required)</t>
+    <t>SHA3-256 (optional)</t>
   </si>
   <si>
     <t>SHA3-256 as defined in FIPS PUP 202</t>
   </si>
   <si>
-    <t>SHA3-384 (required)</t>
+    <t>SHA3-384 (optional)</t>
   </si>
   <si>
     <t>SHA3-384 as defined in FIPS PUP 202</t>
   </si>
   <si>
-    <t>SHA3-512 (required)</t>
+    <t>SHA3-512 (optional)</t>
   </si>
   <si>
     <t>SHA3-512 as defined in FIPS PUP 202</t>
   </si>
   <si>
-    <t>ssdeep (required)</t>
+    <t>ssdeep (optional)</t>
   </si>
   <si>
     <t>ssdeep fuzzy hashing algorithm as defined in the SSDEEP specification</t>
   </si>
   <si>
-    <t>WHIRLPOOL (required)</t>
+    <t>WHIRLPOOL (optional)</t>
   </si>
   <si>
     <t>whirlpool cryptographic hash function as defined in ISO/IEC 10118-3:2004</t>

</xml_diff>

<commit_message>
Add unit tests for attribute and property selectors
</commit_message>
<xml_diff>
--- a/pub-jaen/jaen/schema_gen/openc2_genj.xlsx
+++ b/pub-jaen/jaen/schema_gen/openc2_genj.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="756">
   <si>
-    <t>Generated from schema\openc2.jaen, Tue Apr 11 09:49:57 2017</t>
+    <t>Generated from schema\openc2.jaen, Thu Apr 20 15:52:14 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -690,7 +690,7 @@
     <t>ActuatorSpecifiers</t>
   </si>
   <si>
-    <t>device_id (optional)</t>
+    <t>actuator_id (optional)</t>
   </si>
   <si>
     <t>asset_id (optional)</t>
@@ -1533,7 +1533,7 @@
     <t>Date/time the file was last accessed.</t>
   </si>
   <si>
-    <t>parent-directory (optional)</t>
+    <t>parent_directory (optional)</t>
   </si>
   <si>
     <t>Parent directory of the file.</t>

</xml_diff>